<commit_message>
QB siteyml change 1/21
</commit_message>
<xml_diff>
--- a/Data/ChildTaxCredit.xlsx
+++ b/Data/ChildTaxCredit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmyescanlar/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9BA2BEA-8D06-2A49-B03D-803E6493BF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7B3EA24-3250-B946-A2CE-8E1CDB2D5375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16280" windowHeight="15540" xr2:uid="{3E9CDE0F-FA6F-034A-9811-7F7D1FC042E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
   <si>
     <t>Question</t>
   </si>
@@ -189,9 +189,6 @@
     <t>How many payments have you received so far?</t>
   </si>
   <si>
-    <t>How much did you receive in each payment?</t>
-  </si>
-  <si>
     <t>To what extent has the Child Tax Credit affected your financial situation and how?</t>
   </si>
   <si>
@@ -231,12 +228,6 @@
     <t>69, 71, 73, 81, 83, 85, 87, 89</t>
   </si>
   <si>
-    <t>73, 75, 81, 83, 85, 87, 89</t>
-  </si>
-  <si>
-    <t>83, 85, 87, 89</t>
-  </si>
-  <si>
     <t>Did you receive the monthly Child Tax Credit payments in 2021?</t>
   </si>
   <si>
@@ -245,12 +236,6 @@
 o No, I did not expect to receive them  </t>
   </si>
   <si>
-    <t>67, 69, 73, 81, 83, 85, 87, 89</t>
-  </si>
-  <si>
-    <t>67, 69, 73, 75, 81, 83, 85, 87, 89</t>
-  </si>
-  <si>
     <t>017 Since the Child Tax Credit checks started being sent in July, is your and your family's financial situation…</t>
   </si>
   <si>
@@ -271,13 +256,66 @@
     <t>As you may know, President Biden's administration passed the American Rescue Plan Act, which temporarily increased the Child Tax Credit (CTC) in 2021 to $3,000/year per child age 6-17 and $3,600/year per child age 0-5. Most families received half of their expected 2021 CTC as monthly payments of up to $300/month per child age 0-5 and $250/month per child age 6-17 in July-December 2021.
 These families can receive the second half of their CTC - up to $1,500-$1,800 per child - by filing their taxes in 2022. Families that are eligible but did not receive the monthly payments can get their full benefit - up to $3,000-$3,600 per child - by filing taxes in 2022.
 R3.CTAX.022 How would it impact your family's financial situation if Congress decides not to continue the monthly Child Tax Credit payments?</t>
+  </si>
+  <si>
+    <t>61, 65, 67, 69, 73, 75, 81, 83, 85, 87, 89, 90</t>
+  </si>
+  <si>
+    <t>89, 90</t>
+  </si>
+  <si>
+    <t>How manymonthly payments did you receivebetween July and December, 2021?</t>
+  </si>
+  <si>
+    <t>open ended</t>
+  </si>
+  <si>
+    <t>73, 75, 81, 83, 85, 87, 89, 90</t>
+  </si>
+  <si>
+    <t>How much did you receive in each monthly payment?</t>
+  </si>
+  <si>
+    <r>
+      <t>83, 85, 87, 89</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 90</t>
+    </r>
+  </si>
+  <si>
+    <t>67, 69, 73, 81, 83, 85, 87, 89, 90</t>
+  </si>
+  <si>
+    <t>67, 69, 73, 75, 81, 83, 85, 87, 89, 90</t>
+  </si>
+  <si>
+    <t>67, 69, 73, 75, 90</t>
+  </si>
+  <si>
+    <t>Before the monthly payments began in July 2021, households with children received their Child Tax Credit in one lump sum when they file their taxes. How would you refer to receive your Child Tax Credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o A monthly payment 
+o A lump sum one time per year  </t>
+  </si>
+  <si>
+    <t>87, 90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,6 +367,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -724,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C63828C-283B-A940-8A21-DDF0804D85D3}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -772,21 +818,21 @@
         <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="68">
       <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="5">
-        <v>89</v>
+      <c r="E3" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="F3" s="12"/>
     </row>
@@ -804,7 +850,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="12"/>
     </row>
@@ -822,7 +868,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="12"/>
     </row>
@@ -840,7 +886,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="12"/>
     </row>
@@ -858,7 +904,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="12"/>
     </row>
@@ -876,7 +922,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -1002,7 +1048,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -1020,7 +1066,7 @@
         <v>19</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F17" s="12"/>
     </row>
@@ -1038,7 +1084,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F18" s="12"/>
     </row>
@@ -1056,7 +1102,7 @@
         <v>19</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -1074,7 +1120,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F20" s="12"/>
     </row>
@@ -1092,7 +1138,7 @@
         <v>19</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F21" s="12"/>
     </row>
@@ -1110,182 +1156,210 @@
         <v>19</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" ht="68">
       <c r="A23" s="14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="1:6" ht="34">
+    <row r="24" spans="1:6" ht="51">
       <c r="A24" s="14" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>76</v>
+      </c>
+      <c r="E24" s="5">
+        <v>90</v>
+      </c>
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" ht="34">
       <c r="A25" s="14" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="187">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:6" ht="34">
+      <c r="A26" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" ht="187">
+      <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" ht="51">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" ht="51">
+      <c r="A28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="C28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:6" ht="170">
-      <c r="A28" s="3" t="s">
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" ht="170">
+      <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:6" ht="68">
-      <c r="A29" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="5">
-        <v>89</v>
+      <c r="C29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" spans="1:6" ht="17">
+    <row r="30" spans="1:6" ht="68">
       <c r="A30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="13" t="s">
         <v>57</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6" ht="17">
       <c r="A31" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>58</v>
+        <v>67</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="5">
+        <v>90</v>
       </c>
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" ht="17">
       <c r="A32" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" ht="68">
+    <row r="33" spans="1:6" ht="17">
       <c r="A33" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" ht="17">
       <c r="A34" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>59</v>
+      <c r="E34" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="255">
+    <row r="35" spans="1:6" ht="68">
       <c r="A35" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" ht="17">
+      <c r="A36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="6">
-        <v>89</v>
-      </c>
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="E36" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" ht="255">
+      <c r="A37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="F38" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>